<commit_message>
bug on choice of analyze subject from gendarmes table resolved
</commit_message>
<xml_diff>
--- a/matrice_last.xlsx
+++ b/matrice_last.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bretwalda/PycharmProjects/Matrice_Disciplinaire/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C3746FD-F06E-AC46-85E8-2606B7CB86F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C118A56-510E-0445-96DB-57126280B153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{77F64D44-FC10-C345-B979-7D7A9B227219}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14280" windowHeight="16100" xr2:uid="{77F64D44-FC10-C345-B979-7D7A9B227219}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1774,7 +1774,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1813,13 +1813,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1834,42 +1827,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1894,6 +1851,39 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1925,6 +1915,9 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1939,35 +1932,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3A27F7C7-80CC-C44C-BB61-88EBD47BD9B1}" name="Tableau1" displayName="Tableau1" ref="A1:Z172" totalsRowShown="0" headerRowDxfId="6" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3A27F7C7-80CC-C44C-BB61-88EBD47BD9B1}" name="Tableau1" displayName="Tableau1" ref="A1:Z172" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A1:Z172" xr:uid="{3A27F7C7-80CC-C44C-BB61-88EBD47BD9B1}"/>
   <tableColumns count="26">
-    <tableColumn id="2" xr3:uid="{791B4CAD-E2CC-5D4D-9E02-8E3D26E9D1AC}" name="N° DOSSIER" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{624C1BE3-1E65-824E-8314-9C7A9A6D1F50}" name="ANNEE DE PUNITION" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{D7538FFB-D5EA-444E-B20A-E255383ECF68}" name="N° ORDRE" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{06B6C37E-7BD7-F44A-93E7-4AC19CEAE9D6}" name="DATE ENR" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{4AD808A8-DAEF-6049-ADF0-F580AE391DC1}" name="MLE" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{A8C9E3F5-752C-B94C-A604-97D8BDB5243F}" name="NOM ET PRENOMS" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{DFEDC5BD-6789-D94D-967C-2C11B268C022}" name="GRADE" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{5DFE2027-2A7C-4541-A7B9-8BE001A99782}" name="SEXE" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{A7340386-17E8-1C48-B1F1-0635EF346251}" name="DATE DE NAISSANCE" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{E84FDAAD-CBE0-B541-95EE-2CA64D99257B}" name="AGE" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{3503C267-2E0C-4844-8CB7-074AA4EC3E80}" name="UNITE" dataDxfId="2"/>
-    <tableColumn id="17" xr3:uid="{7808847B-2017-D046-99D6-DBA47699F811}" name="LEGIONS" dataDxfId="4"/>
-    <tableColumn id="18" xr3:uid="{326A5373-14F0-D749-8267-844918F89DD6}" name="SUBDIV" dataDxfId="5"/>
-    <tableColumn id="19" xr3:uid="{C051AB43-5DD9-C647-9362-6B5ED058223C}" name="REGIONS" dataDxfId="19"/>
-    <tableColumn id="20" xr3:uid="{AB351E8F-585C-B04F-99CA-7912CE207E60}" name="DATE D'ENTREE GIE" dataDxfId="18"/>
-    <tableColumn id="21" xr3:uid="{8DBB8600-AA68-B64A-AD2E-5338D6E66B64}" name="ANNEE DE SERVICE" dataDxfId="17"/>
-    <tableColumn id="22" xr3:uid="{AC89039D-AA93-9F4F-A2DE-F07FF36B9FFC}" name="SITUATION MATRIMONIALE" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{791B4CAD-E2CC-5D4D-9E02-8E3D26E9D1AC}" name="N° DOSSIER" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{624C1BE3-1E65-824E-8314-9C7A9A6D1F50}" name="ANNEE DE PUNITION" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{D7538FFB-D5EA-444E-B20A-E255383ECF68}" name="N° ORDRE" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{06B6C37E-7BD7-F44A-93E7-4AC19CEAE9D6}" name="DATE ENR" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{4AD808A8-DAEF-6049-ADF0-F580AE391DC1}" name="MLE" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{A8C9E3F5-752C-B94C-A604-97D8BDB5243F}" name="NOM ET PRENOMS" dataDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{DFEDC5BD-6789-D94D-967C-2C11B268C022}" name="GRADE" dataDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{5DFE2027-2A7C-4541-A7B9-8BE001A99782}" name="SEXE" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{A7340386-17E8-1C48-B1F1-0635EF346251}" name="DATE DE NAISSANCE" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{E84FDAAD-CBE0-B541-95EE-2CA64D99257B}" name="AGE" dataDxfId="17"/>
+    <tableColumn id="13" xr3:uid="{3503C267-2E0C-4844-8CB7-074AA4EC3E80}" name="UNITE" dataDxfId="16"/>
+    <tableColumn id="17" xr3:uid="{7808847B-2017-D046-99D6-DBA47699F811}" name="LEGIONS" dataDxfId="15"/>
+    <tableColumn id="18" xr3:uid="{326A5373-14F0-D749-8267-844918F89DD6}" name="SUBDIV" dataDxfId="14"/>
+    <tableColumn id="19" xr3:uid="{C051AB43-5DD9-C647-9362-6B5ED058223C}" name="REGIONS" dataDxfId="13"/>
+    <tableColumn id="20" xr3:uid="{AB351E8F-585C-B04F-99CA-7912CE207E60}" name="DATE D'ENTREE GIE" dataDxfId="12"/>
+    <tableColumn id="21" xr3:uid="{8DBB8600-AA68-B64A-AD2E-5338D6E66B64}" name="ANNEE DE SERVICE" dataDxfId="11"/>
+    <tableColumn id="22" xr3:uid="{AC89039D-AA93-9F4F-A2DE-F07FF36B9FFC}" name="SITUATION MATRIMONIALE" dataDxfId="10"/>
     <tableColumn id="23" xr3:uid="{0665EB1D-997E-EC4B-9923-A037E72466A4}" name="NB ENF" dataDxfId="9"/>
-    <tableColumn id="24" xr3:uid="{DD9881FB-BD45-724F-8289-AC59D0EB15DF}" name="FAUTE COMMISE" dataDxfId="7"/>
-    <tableColumn id="25" xr3:uid="{EF2B1D03-4D30-F645-86E7-819960278C4E}" name="DATE DES FAITS" dataDxfId="8"/>
-    <tableColumn id="26" xr3:uid="{018A27F6-5D4E-5E41-A0DD-92B979206BB7}" name="N° CAT" dataDxfId="15"/>
-    <tableColumn id="27" xr3:uid="{3E5B99A5-8AFA-1640-8B63-53E3391CC84C}" name="STATUT" dataDxfId="14"/>
-    <tableColumn id="28" xr3:uid="{6B4396D6-BD64-1A41-8AF1-F5B961F9F82A}" name="REFERENCE DU STATUT" dataDxfId="13"/>
-    <tableColumn id="29" xr3:uid="{8B9E5E42-A12C-DF44-946F-E9BC418413C1}" name="TAUX (JAR)" dataDxfId="12"/>
-    <tableColumn id="30" xr3:uid="{9E0F2322-A286-644E-B5B6-F533B974CE39}" name="COMITE" dataDxfId="11"/>
-    <tableColumn id="31" xr3:uid="{F36FADD0-10D0-7846-9F7F-8996F5863537}" name="ANNEE DES FAITS" dataDxfId="10"/>
+    <tableColumn id="24" xr3:uid="{DD9881FB-BD45-724F-8289-AC59D0EB15DF}" name="FAUTE COMMISE" dataDxfId="8"/>
+    <tableColumn id="25" xr3:uid="{EF2B1D03-4D30-F645-86E7-819960278C4E}" name="DATE DES FAITS" dataDxfId="7"/>
+    <tableColumn id="26" xr3:uid="{018A27F6-5D4E-5E41-A0DD-92B979206BB7}" name="N° CAT" dataDxfId="6"/>
+    <tableColumn id="27" xr3:uid="{3E5B99A5-8AFA-1640-8B63-53E3391CC84C}" name="STATUT" dataDxfId="5"/>
+    <tableColumn id="28" xr3:uid="{6B4396D6-BD64-1A41-8AF1-F5B961F9F82A}" name="REFERENCE DU STATUT" dataDxfId="4"/>
+    <tableColumn id="29" xr3:uid="{8B9E5E42-A12C-DF44-946F-E9BC418413C1}" name="TAUX (JAR)" dataDxfId="3"/>
+    <tableColumn id="30" xr3:uid="{9E0F2322-A286-644E-B5B6-F533B974CE39}" name="COMITE" dataDxfId="2"/>
+    <tableColumn id="31" xr3:uid="{F36FADD0-10D0-7846-9F7F-8996F5863537}" name="ANNEE DES FAITS" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2272,8 +2265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F271C14-EBED-F84E-90DF-367173903928}">
   <dimension ref="A1:Z172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F138" workbookViewId="0">
-      <selection activeCell="B174" sqref="B174"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2284,7 +2277,6 @@
     <col min="6" max="6" width="42" style="4" customWidth="1"/>
     <col min="7" max="7" width="11.3984375" customWidth="1"/>
     <col min="9" max="9" width="12.796875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11" style="16"/>
     <col min="11" max="11" width="39.3984375" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="25.19921875" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.796875" customWidth="1"/>
@@ -2331,7 +2323,7 @@
       <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="7" t="s">
         <v>8</v>
       </c>
       <c r="K1" s="9" t="s">
@@ -2411,7 +2403,7 @@
       <c r="I2" s="3">
         <v>30028</v>
       </c>
-      <c r="J2" s="15">
+      <c r="J2" s="2">
         <v>41</v>
       </c>
       <c r="K2" s="5" t="s">
@@ -2491,7 +2483,7 @@
       <c r="I3" s="3">
         <v>34455</v>
       </c>
-      <c r="J3" s="15">
+      <c r="J3" s="2">
         <v>28</v>
       </c>
       <c r="K3" s="5" t="s">
@@ -2571,7 +2563,7 @@
       <c r="I4" s="3">
         <v>35959</v>
       </c>
-      <c r="J4" s="15">
+      <c r="J4" s="2">
         <v>24</v>
       </c>
       <c r="K4" s="5" t="s">
@@ -2651,7 +2643,7 @@
       <c r="I5" s="3">
         <v>28477</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="2">
         <v>45</v>
       </c>
       <c r="K5" s="5" t="s">
@@ -2731,7 +2723,7 @@
       <c r="I6" s="3">
         <v>36119</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="2">
         <v>25</v>
       </c>
       <c r="K6" s="5" t="s">
@@ -2811,7 +2803,7 @@
       <c r="I7" s="3">
         <v>33292</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="2">
         <v>32</v>
       </c>
       <c r="K7" s="5" t="s">
@@ -2891,7 +2883,7 @@
       <c r="I8" s="3">
         <v>36289</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="2">
         <v>24</v>
       </c>
       <c r="K8" s="5" t="s">
@@ -2971,7 +2963,7 @@
       <c r="I9" s="3">
         <v>32249</v>
       </c>
-      <c r="J9" s="15">
+      <c r="J9" s="2">
         <v>35</v>
       </c>
       <c r="K9" s="5" t="s">
@@ -3051,8 +3043,8 @@
       <c r="I10" s="3">
         <v>1</v>
       </c>
-      <c r="J10" s="15" t="e">
-        <v>#VALUE!</v>
+      <c r="J10" s="2">
+        <v>0</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>68</v>
@@ -3131,7 +3123,7 @@
       <c r="I11" s="3">
         <v>27867</v>
       </c>
-      <c r="J11" s="15">
+      <c r="J11" s="2">
         <v>47</v>
       </c>
       <c r="K11" s="5" t="s">
@@ -3211,7 +3203,7 @@
       <c r="I12" s="3">
         <v>31554</v>
       </c>
-      <c r="J12" s="15">
+      <c r="J12" s="2">
         <v>37</v>
       </c>
       <c r="K12" s="5" t="s">
@@ -3291,7 +3283,7 @@
       <c r="I13" s="3">
         <v>34447</v>
       </c>
-      <c r="J13" s="15">
+      <c r="J13" s="2">
         <v>28</v>
       </c>
       <c r="K13" s="5" t="s">
@@ -3371,7 +3363,7 @@
       <c r="I14" s="3">
         <v>36711</v>
       </c>
-      <c r="J14" s="15">
+      <c r="J14" s="2">
         <v>22</v>
       </c>
       <c r="K14" s="5" t="s">
@@ -3451,7 +3443,7 @@
       <c r="I15" s="3">
         <v>1</v>
       </c>
-      <c r="J15" s="15">
+      <c r="J15" s="2">
         <v>123</v>
       </c>
       <c r="K15" s="5" t="s">
@@ -3531,7 +3523,7 @@
       <c r="I16" s="3">
         <v>36570</v>
       </c>
-      <c r="J16" s="15">
+      <c r="J16" s="2">
         <v>23</v>
       </c>
       <c r="K16" s="5" t="s">
@@ -3611,7 +3603,7 @@
       <c r="I17" s="3">
         <v>27740</v>
       </c>
-      <c r="J17" s="15">
+      <c r="J17" s="2">
         <v>47</v>
       </c>
       <c r="K17" s="5" t="s">
@@ -3691,7 +3683,7 @@
       <c r="I18" s="3">
         <v>26531</v>
       </c>
-      <c r="J18" s="15">
+      <c r="J18" s="2">
         <v>51</v>
       </c>
       <c r="K18" s="5" t="s">
@@ -3771,7 +3763,7 @@
       <c r="I19" s="3">
         <v>32516</v>
       </c>
-      <c r="J19" s="15">
+      <c r="J19" s="2">
         <v>34</v>
       </c>
       <c r="K19" s="5" t="s">
@@ -3851,7 +3843,7 @@
       <c r="I20" s="3">
         <v>34257</v>
       </c>
-      <c r="J20" s="15">
+      <c r="J20" s="2">
         <v>30</v>
       </c>
       <c r="K20" s="5" t="s">
@@ -3931,7 +3923,7 @@
       <c r="I21" s="3">
         <v>34912</v>
       </c>
-      <c r="J21" s="15">
+      <c r="J21" s="2">
         <v>28</v>
       </c>
       <c r="K21" s="5" t="s">
@@ -4011,7 +4003,7 @@
       <c r="I22" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="J22" s="15">
+      <c r="J22" s="2">
         <v>38</v>
       </c>
       <c r="K22" s="5" t="s">
@@ -4091,7 +4083,7 @@
       <c r="I23" s="3">
         <v>32822</v>
       </c>
-      <c r="J23" s="15">
+      <c r="J23" s="2">
         <v>30</v>
       </c>
       <c r="K23" s="5" t="s">
@@ -4171,7 +4163,7 @@
       <c r="I24" s="3">
         <v>34212</v>
       </c>
-      <c r="J24" s="15">
+      <c r="J24" s="2">
         <v>30</v>
       </c>
       <c r="K24" s="5" t="s">
@@ -4251,7 +4243,7 @@
       <c r="I25" s="3">
         <v>33237</v>
       </c>
-      <c r="J25" s="15">
+      <c r="J25" s="2">
         <v>32</v>
       </c>
       <c r="K25" s="5" t="s">
@@ -4331,7 +4323,7 @@
       <c r="I26" s="3">
         <v>36537</v>
       </c>
-      <c r="J26" s="15">
+      <c r="J26" s="2">
         <v>23</v>
       </c>
       <c r="K26" s="5" t="s">
@@ -4411,7 +4403,7 @@
       <c r="I27" s="3">
         <v>33193</v>
       </c>
-      <c r="J27" s="15">
+      <c r="J27" s="2">
         <v>32</v>
       </c>
       <c r="K27" s="5" t="s">
@@ -4491,7 +4483,7 @@
       <c r="I28" s="3">
         <v>32308</v>
       </c>
-      <c r="J28" s="15">
+      <c r="J28" s="2">
         <v>35</v>
       </c>
       <c r="K28" s="5" t="s">
@@ -4571,7 +4563,7 @@
       <c r="I29" s="3">
         <v>30403</v>
       </c>
-      <c r="J29" s="15">
+      <c r="J29" s="2">
         <v>40</v>
       </c>
       <c r="K29" s="5" t="s">
@@ -4651,7 +4643,7 @@
       <c r="I30" s="3">
         <v>32502</v>
       </c>
-      <c r="J30" s="15">
+      <c r="J30" s="2">
         <v>35</v>
       </c>
       <c r="K30" s="5" t="s">
@@ -4731,7 +4723,7 @@
       <c r="I31" s="3">
         <v>35152</v>
       </c>
-      <c r="J31" s="15">
+      <c r="J31" s="2">
         <v>26</v>
       </c>
       <c r="K31" s="5" t="s">
@@ -4811,7 +4803,7 @@
       <c r="I32" s="3">
         <v>36375</v>
       </c>
-      <c r="J32" s="15">
+      <c r="J32" s="2">
         <v>23</v>
       </c>
       <c r="K32" s="5" t="s">
@@ -4891,7 +4883,7 @@
       <c r="I33" s="3">
         <v>35057</v>
       </c>
-      <c r="J33" s="15">
+      <c r="J33" s="2">
         <v>27</v>
       </c>
       <c r="K33" s="5" t="s">
@@ -4971,7 +4963,7 @@
       <c r="I34" s="3">
         <v>37273</v>
       </c>
-      <c r="J34" s="15">
+      <c r="J34" s="2">
         <v>21</v>
       </c>
       <c r="K34" s="5" t="s">
@@ -5051,7 +5043,7 @@
       <c r="I35" s="3">
         <v>36967</v>
       </c>
-      <c r="J35" s="15">
+      <c r="J35" s="2">
         <v>22</v>
       </c>
       <c r="K35" s="5" t="s">
@@ -5131,7 +5123,7 @@
       <c r="I36" s="3">
         <v>29233</v>
       </c>
-      <c r="J36" s="15">
+      <c r="J36" s="2">
         <v>43</v>
       </c>
       <c r="K36" s="5" t="s">
@@ -5211,7 +5203,7 @@
       <c r="I37" s="3">
         <v>32841</v>
       </c>
-      <c r="J37" s="15">
+      <c r="J37" s="2">
         <v>33</v>
       </c>
       <c r="K37" s="5" t="s">
@@ -5291,7 +5283,7 @@
       <c r="I38" s="3">
         <v>27777</v>
       </c>
-      <c r="J38" s="15">
+      <c r="J38" s="2">
         <v>47</v>
       </c>
       <c r="K38" s="5" t="s">
@@ -5371,7 +5363,7 @@
       <c r="I39" s="3">
         <v>26663</v>
       </c>
-      <c r="J39" s="15">
+      <c r="J39" s="2">
         <v>50</v>
       </c>
       <c r="K39" s="5" t="s">
@@ -5451,7 +5443,7 @@
       <c r="I40" s="3">
         <v>1</v>
       </c>
-      <c r="J40" s="15">
+      <c r="J40" s="2">
         <v>123</v>
       </c>
       <c r="K40" s="5" t="s">
@@ -5531,7 +5523,7 @@
       <c r="I41" s="3">
         <v>34907</v>
       </c>
-      <c r="J41" s="15">
+      <c r="J41" s="2">
         <v>28</v>
       </c>
       <c r="K41" s="5" t="s">
@@ -5611,7 +5603,7 @@
       <c r="I42" s="3">
         <v>26665</v>
       </c>
-      <c r="J42" s="15">
+      <c r="J42" s="2">
         <v>51</v>
       </c>
       <c r="K42" s="5" t="s">
@@ -5691,7 +5683,7 @@
       <c r="I43" s="3">
         <v>27177</v>
       </c>
-      <c r="J43" s="15">
+      <c r="J43" s="2">
         <v>49</v>
       </c>
       <c r="K43" s="5" t="s">
@@ -5771,7 +5763,7 @@
       <c r="I44" s="3">
         <v>30320</v>
       </c>
-      <c r="J44" s="15">
+      <c r="J44" s="2">
         <v>40</v>
       </c>
       <c r="K44" s="5" t="s">
@@ -5851,7 +5843,7 @@
       <c r="I45" s="3">
         <v>30280</v>
       </c>
-      <c r="J45" s="15">
+      <c r="J45" s="2">
         <v>41</v>
       </c>
       <c r="K45" s="5" t="s">
@@ -5931,7 +5923,7 @@
       <c r="I46" s="3">
         <v>30163</v>
       </c>
-      <c r="J46" s="15">
+      <c r="J46" s="2">
         <v>41</v>
       </c>
       <c r="K46" s="5" t="s">
@@ -6011,7 +6003,7 @@
       <c r="I47" s="3">
         <v>36154</v>
       </c>
-      <c r="J47" s="15">
+      <c r="J47" s="2">
         <v>24</v>
       </c>
       <c r="K47" s="5" t="s">
@@ -6091,7 +6083,7 @@
       <c r="I48" s="3">
         <v>31028</v>
       </c>
-      <c r="J48" s="15">
+      <c r="J48" s="2">
         <v>37</v>
       </c>
       <c r="K48" s="5" t="s">
@@ -6171,7 +6163,7 @@
       <c r="I49" s="3">
         <v>1</v>
       </c>
-      <c r="J49" s="15">
+      <c r="J49" s="2">
         <v>123</v>
       </c>
       <c r="K49" s="5" t="s">
@@ -6251,7 +6243,7 @@
       <c r="I50" s="3">
         <v>27883</v>
       </c>
-      <c r="J50" s="15">
+      <c r="J50" s="2">
         <v>47</v>
       </c>
       <c r="K50" s="5" t="s">
@@ -6331,7 +6323,7 @@
       <c r="I51" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="J51" s="15">
+      <c r="J51" s="2">
         <v>38</v>
       </c>
       <c r="K51" s="5" t="s">
@@ -6411,7 +6403,7 @@
       <c r="I52" s="3">
         <v>1</v>
       </c>
-      <c r="J52" s="15">
+      <c r="J52" s="2">
         <v>123</v>
       </c>
       <c r="K52" s="5" t="s">
@@ -6491,7 +6483,7 @@
       <c r="I53" s="3">
         <v>36114</v>
       </c>
-      <c r="J53" s="15">
+      <c r="J53" s="2">
         <v>25</v>
       </c>
       <c r="K53" s="5" t="s">
@@ -6571,7 +6563,7 @@
       <c r="I54" s="3">
         <v>32476</v>
       </c>
-      <c r="J54" s="15">
+      <c r="J54" s="2">
         <v>34</v>
       </c>
       <c r="K54" s="5" t="s">
@@ -6651,7 +6643,7 @@
       <c r="I55" s="3">
         <v>32567</v>
       </c>
-      <c r="J55" s="15">
+      <c r="J55" s="2">
         <v>34</v>
       </c>
       <c r="K55" s="5" t="s">
@@ -6731,7 +6723,7 @@
       <c r="I56" s="3">
         <v>36203</v>
       </c>
-      <c r="J56" s="15">
+      <c r="J56" s="2">
         <v>25</v>
       </c>
       <c r="K56" s="5" t="s">
@@ -6811,7 +6803,7 @@
       <c r="I57" s="3">
         <v>29937</v>
       </c>
-      <c r="J57" s="15">
+      <c r="J57" s="2">
         <v>41</v>
       </c>
       <c r="K57" s="5" t="s">
@@ -6891,7 +6883,7 @@
       <c r="I58" s="3">
         <v>34625</v>
       </c>
-      <c r="J58" s="15">
+      <c r="J58" s="2">
         <v>29</v>
       </c>
       <c r="K58" s="5" t="s">
@@ -6971,7 +6963,7 @@
       <c r="I59" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="15">
+      <c r="J59" s="2">
         <v>40</v>
       </c>
       <c r="K59" s="5" t="s">
@@ -7051,7 +7043,7 @@
       <c r="I60" s="3">
         <v>31968</v>
       </c>
-      <c r="J60" s="15">
+      <c r="J60" s="2">
         <v>37</v>
       </c>
       <c r="K60" s="5" t="s">
@@ -7131,7 +7123,7 @@
       <c r="I61" s="3">
         <v>32979</v>
       </c>
-      <c r="J61" s="15">
+      <c r="J61" s="2">
         <v>33</v>
       </c>
       <c r="K61" s="5" t="s">
@@ -7211,7 +7203,7 @@
       <c r="I62" s="3">
         <v>37504</v>
       </c>
-      <c r="J62" s="15">
+      <c r="J62" s="2">
         <v>21</v>
       </c>
       <c r="K62" s="5" t="s">
@@ -7291,7 +7283,7 @@
       <c r="I63" s="3">
         <v>36317</v>
       </c>
-      <c r="J63" s="15">
+      <c r="J63" s="2">
         <v>24</v>
       </c>
       <c r="K63" s="5" t="s">
@@ -7371,7 +7363,7 @@
       <c r="I64" s="3">
         <v>36395</v>
       </c>
-      <c r="J64" s="15">
+      <c r="J64" s="2">
         <v>24</v>
       </c>
       <c r="K64" s="5" t="s">
@@ -7451,7 +7443,7 @@
       <c r="I65" s="3">
         <v>35066</v>
       </c>
-      <c r="J65" s="15">
+      <c r="J65" s="2">
         <v>28</v>
       </c>
       <c r="K65" s="5" t="s">
@@ -7531,7 +7523,7 @@
       <c r="I66" s="3">
         <v>35480</v>
       </c>
-      <c r="J66" s="15">
+      <c r="J66" s="2">
         <v>27</v>
       </c>
       <c r="K66" s="5" t="s">
@@ -7611,7 +7603,7 @@
       <c r="I67" s="3">
         <v>36301</v>
       </c>
-      <c r="J67" s="15">
+      <c r="J67" s="2">
         <v>24</v>
       </c>
       <c r="K67" s="5" t="s">
@@ -7691,7 +7683,7 @@
       <c r="I68" s="3">
         <v>37426</v>
       </c>
-      <c r="J68" s="15">
+      <c r="J68" s="2">
         <v>21</v>
       </c>
       <c r="K68" s="5" t="s">
@@ -7771,7 +7763,7 @@
       <c r="I69" s="3">
         <v>30431</v>
       </c>
-      <c r="J69" s="15">
+      <c r="J69" s="2">
         <v>40</v>
       </c>
       <c r="K69" s="5" t="s">
@@ -7851,7 +7843,7 @@
       <c r="I70" s="3">
         <v>27926</v>
       </c>
-      <c r="J70" s="15">
+      <c r="J70" s="2">
         <v>33</v>
       </c>
       <c r="K70" s="5" t="s">
@@ -7931,7 +7923,7 @@
       <c r="I71" s="3">
         <v>35525</v>
       </c>
-      <c r="J71" s="15">
+      <c r="J71" s="2">
         <v>26</v>
       </c>
       <c r="K71" s="5" t="s">
@@ -8011,7 +8003,7 @@
       <c r="I72" s="3">
         <v>35796</v>
       </c>
-      <c r="J72" s="15">
+      <c r="J72" s="2">
         <v>26</v>
       </c>
       <c r="K72" s="5" t="s">
@@ -8091,7 +8083,7 @@
       <c r="I73" s="3">
         <v>32424</v>
       </c>
-      <c r="J73" s="15">
+      <c r="J73" s="2">
         <v>35</v>
       </c>
       <c r="K73" s="5" t="s">
@@ -8171,7 +8163,7 @@
       <c r="I74" s="3">
         <v>26989</v>
       </c>
-      <c r="J74" s="15">
+      <c r="J74" s="2">
         <v>46</v>
       </c>
       <c r="K74" s="5" t="s">
@@ -8251,7 +8243,7 @@
       <c r="I75" s="3">
         <v>32523</v>
       </c>
-      <c r="J75" s="15">
+      <c r="J75" s="2">
         <v>35</v>
       </c>
       <c r="K75" s="5" t="s">
@@ -8331,7 +8323,7 @@
       <c r="I76" s="3">
         <v>26557</v>
       </c>
-      <c r="J76" s="15">
+      <c r="J76" s="2">
         <v>44</v>
       </c>
       <c r="K76" s="5" t="s">
@@ -8409,7 +8401,7 @@
       <c r="I77" s="3">
         <v>27873</v>
       </c>
-      <c r="J77" s="15">
+      <c r="J77" s="2">
         <v>47</v>
       </c>
       <c r="K77" s="5" t="s">
@@ -8487,7 +8479,7 @@
       <c r="I78" s="3">
         <v>27746</v>
       </c>
-      <c r="J78" s="15">
+      <c r="J78" s="2">
         <v>51</v>
       </c>
       <c r="K78" s="5" t="s">
@@ -8567,7 +8559,7 @@
       <c r="I79" s="3">
         <v>32872</v>
       </c>
-      <c r="J79" s="15">
+      <c r="J79" s="2">
         <v>42</v>
       </c>
       <c r="K79" s="5" t="s">
@@ -8647,7 +8639,7 @@
       <c r="I80" s="3">
         <v>29566</v>
       </c>
-      <c r="J80" s="15">
+      <c r="J80" s="2">
         <v>34</v>
       </c>
       <c r="K80" s="5" t="s">
@@ -8727,7 +8719,7 @@
       <c r="I81" s="3">
         <v>29828</v>
       </c>
-      <c r="J81" s="15">
+      <c r="J81" s="2">
         <v>42</v>
       </c>
       <c r="K81" s="5" t="s">
@@ -8807,7 +8799,7 @@
       <c r="I82" s="3">
         <v>35270</v>
       </c>
-      <c r="J82" s="15">
+      <c r="J82" s="2">
         <v>27</v>
       </c>
       <c r="K82" s="5" t="s">
@@ -8887,7 +8879,7 @@
       <c r="I83" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="J83" s="15">
+      <c r="J83" s="2">
         <v>38</v>
       </c>
       <c r="K83" s="5" t="s">
@@ -8967,7 +8959,7 @@
       <c r="I84" s="3">
         <v>30676</v>
       </c>
-      <c r="J84" s="15">
+      <c r="J84" s="2">
         <v>40</v>
       </c>
       <c r="K84" s="5" t="s">
@@ -9047,7 +9039,7 @@
       <c r="I85" s="3">
         <v>31944</v>
       </c>
-      <c r="J85" s="15">
+      <c r="J85" s="2">
         <v>36</v>
       </c>
       <c r="K85" s="5" t="s">
@@ -9125,7 +9117,7 @@
       <c r="I86" s="3">
         <v>33381</v>
       </c>
-      <c r="J86" s="15">
+      <c r="J86" s="2">
         <v>32</v>
       </c>
       <c r="K86" s="5" t="s">
@@ -9203,7 +9195,7 @@
       <c r="I87" s="3">
         <v>26662</v>
       </c>
-      <c r="J87" s="15">
+      <c r="J87" s="2">
         <v>51</v>
       </c>
       <c r="K87" s="5" t="s">
@@ -9283,7 +9275,7 @@
       <c r="I88" s="3">
         <v>28004</v>
       </c>
-      <c r="J88" s="15">
+      <c r="J88" s="2">
         <v>47</v>
       </c>
       <c r="K88" s="5" t="s">
@@ -9363,7 +9355,7 @@
       <c r="I89" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="J89" s="15">
+      <c r="J89" s="2">
         <v>39</v>
       </c>
       <c r="K89" s="5" t="s">
@@ -9443,7 +9435,7 @@
       <c r="I90" s="3">
         <v>31057</v>
       </c>
-      <c r="J90" s="15">
+      <c r="J90" s="2">
         <v>38</v>
       </c>
       <c r="K90" s="5" t="s">
@@ -9523,7 +9515,7 @@
       <c r="I91" s="3">
         <v>30090</v>
       </c>
-      <c r="J91" s="15">
+      <c r="J91" s="2">
         <v>41</v>
       </c>
       <c r="K91" s="5" t="s">
@@ -9603,7 +9595,7 @@
       <c r="I92" s="3">
         <v>1</v>
       </c>
-      <c r="J92" s="15">
+      <c r="J92" s="2">
         <v>123</v>
       </c>
       <c r="K92" s="5" t="s">
@@ -9683,7 +9675,7 @@
       <c r="I93" s="3">
         <v>36160</v>
       </c>
-      <c r="J93" s="15">
+      <c r="J93" s="2">
         <v>25</v>
       </c>
       <c r="K93" s="5" t="s">
@@ -9763,7 +9755,7 @@
       <c r="I94" s="3">
         <v>31148</v>
       </c>
-      <c r="J94" s="15">
+      <c r="J94" s="2">
         <v>38</v>
       </c>
       <c r="K94" s="5" t="s">
@@ -9843,7 +9835,7 @@
       <c r="I95" s="3">
         <v>1</v>
       </c>
-      <c r="J95" s="15">
+      <c r="J95" s="2">
         <v>124</v>
       </c>
       <c r="K95" s="5" t="s">
@@ -9921,7 +9913,7 @@
       <c r="I96" s="3">
         <v>32630</v>
       </c>
-      <c r="J96" s="15">
+      <c r="J96" s="2">
         <v>34</v>
       </c>
       <c r="K96" s="5" t="s">
@@ -9997,7 +9989,7 @@
       <c r="I97" s="3">
         <v>34179</v>
       </c>
-      <c r="J97" s="15">
+      <c r="J97" s="2">
         <v>30</v>
       </c>
       <c r="K97" s="5" t="s">
@@ -10073,7 +10065,7 @@
       <c r="I98" s="3">
         <v>36786</v>
       </c>
-      <c r="J98" s="15">
+      <c r="J98" s="2">
         <v>23</v>
       </c>
       <c r="K98" s="5" t="s">
@@ -10149,7 +10141,7 @@
       <c r="I99" s="3">
         <v>35649</v>
       </c>
-      <c r="J99" s="15">
+      <c r="J99" s="2">
         <v>26</v>
       </c>
       <c r="K99" s="5" t="s">
@@ -10227,7 +10219,7 @@
       <c r="I100" s="3">
         <v>26136</v>
       </c>
-      <c r="J100" s="15">
+      <c r="J100" s="2">
         <v>52</v>
       </c>
       <c r="K100" s="5" t="s">
@@ -10307,7 +10299,7 @@
       <c r="I101" s="3">
         <v>35002</v>
       </c>
-      <c r="J101" s="15">
+      <c r="J101" s="2">
         <v>28</v>
       </c>
       <c r="K101" s="5" t="s">
@@ -10387,7 +10379,7 @@
       <c r="I102" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="J102" s="15">
+      <c r="J102" s="2">
         <v>35</v>
       </c>
       <c r="K102" s="5" t="s">
@@ -10467,7 +10459,7 @@
       <c r="I103" s="3">
         <v>32605</v>
       </c>
-      <c r="J103" s="15">
+      <c r="J103" s="2">
         <v>34</v>
       </c>
       <c r="K103" s="5" t="s">
@@ -10547,7 +10539,7 @@
       <c r="I104" s="3">
         <v>32715</v>
       </c>
-      <c r="J104" s="15">
+      <c r="J104" s="2">
         <v>40</v>
       </c>
       <c r="K104" s="5" t="s">
@@ -10627,7 +10619,7 @@
       <c r="I105" s="3">
         <v>32847</v>
       </c>
-      <c r="J105" s="15">
+      <c r="J105" s="2">
         <v>34</v>
       </c>
       <c r="K105" s="5" t="s">
@@ -10707,7 +10699,7 @@
       <c r="I106" s="3">
         <v>31572</v>
       </c>
-      <c r="J106" s="15">
+      <c r="J106" s="2">
         <v>37</v>
       </c>
       <c r="K106" s="5" t="s">
@@ -10787,7 +10779,7 @@
       <c r="I107" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="J107" s="15">
+      <c r="J107" s="2">
         <v>43</v>
       </c>
       <c r="K107" s="5" t="s">
@@ -10867,7 +10859,7 @@
       <c r="I108" s="3">
         <v>35211</v>
       </c>
-      <c r="J108" s="15">
+      <c r="J108" s="2">
         <v>28</v>
       </c>
       <c r="K108" s="5" t="s">
@@ -10947,7 +10939,7 @@
       <c r="I109" s="3">
         <v>32661</v>
       </c>
-      <c r="J109" s="15">
+      <c r="J109" s="2">
         <v>34</v>
       </c>
       <c r="K109" s="5" t="s">
@@ -11027,7 +11019,7 @@
       <c r="I110" s="3">
         <v>32874</v>
       </c>
-      <c r="J110" s="15">
+      <c r="J110" s="2">
         <v>33</v>
       </c>
       <c r="K110" s="5" t="s">
@@ -11107,7 +11099,7 @@
       <c r="I111" s="3">
         <v>27382</v>
       </c>
-      <c r="J111" s="15">
+      <c r="J111" s="2">
         <v>44</v>
       </c>
       <c r="K111" s="5" t="s">
@@ -11187,7 +11179,7 @@
       <c r="I112" s="3">
         <v>35922</v>
       </c>
-      <c r="J112" s="15">
+      <c r="J112" s="2">
         <v>26</v>
       </c>
       <c r="K112" s="5" t="s">
@@ -11267,7 +11259,7 @@
       <c r="I113" s="3">
         <v>36486</v>
       </c>
-      <c r="J113" s="15">
+      <c r="J113" s="2">
         <v>24</v>
       </c>
       <c r="K113" s="5" t="s">
@@ -11347,7 +11339,7 @@
       <c r="I114" s="3">
         <v>36532</v>
       </c>
-      <c r="J114" s="15">
+      <c r="J114" s="2">
         <v>24</v>
       </c>
       <c r="K114" s="5" t="s">
@@ -11425,7 +11417,7 @@
       <c r="I115" s="3">
         <v>30808</v>
       </c>
-      <c r="J115" s="15">
+      <c r="J115" s="2">
         <v>37</v>
       </c>
       <c r="K115" s="5" t="s">
@@ -11505,7 +11497,7 @@
       <c r="I116" s="3">
         <v>32169</v>
       </c>
-      <c r="J116" s="15">
+      <c r="J116" s="2">
         <v>36</v>
       </c>
       <c r="K116" s="5" t="s">
@@ -11583,7 +11575,7 @@
       <c r="I117" s="3">
         <v>36514</v>
       </c>
-      <c r="J117" s="15">
+      <c r="J117" s="2">
         <v>24</v>
       </c>
       <c r="K117" s="5" t="s">
@@ -11661,7 +11653,7 @@
       <c r="I118" s="3">
         <v>35152</v>
       </c>
-      <c r="J118" s="15">
+      <c r="J118" s="2">
         <v>27</v>
       </c>
       <c r="K118" s="5" t="s">
@@ -11739,7 +11731,7 @@
       <c r="I119" s="3">
         <v>32791</v>
       </c>
-      <c r="J119" s="15">
+      <c r="J119" s="2">
         <v>29</v>
       </c>
       <c r="K119" s="5" t="s">
@@ -11817,7 +11809,7 @@
       <c r="I120" s="3">
         <v>26946</v>
       </c>
-      <c r="J120" s="15">
+      <c r="J120" s="2">
         <v>50</v>
       </c>
       <c r="K120" s="5" t="s">
@@ -11895,7 +11887,7 @@
       <c r="I121" s="3">
         <v>28090</v>
       </c>
-      <c r="J121" s="15">
+      <c r="J121" s="2">
         <v>46</v>
       </c>
       <c r="K121" s="5" t="s">
@@ -11975,7 +11967,7 @@
       <c r="I122" s="3">
         <v>37842</v>
       </c>
-      <c r="J122" s="15">
+      <c r="J122" s="2">
         <v>20</v>
       </c>
       <c r="K122" s="5" t="s">
@@ -12053,7 +12045,7 @@
       <c r="I123" s="3">
         <v>29581</v>
       </c>
-      <c r="J123" s="15">
+      <c r="J123" s="2">
         <v>43</v>
       </c>
       <c r="K123" s="5" t="s">
@@ -12133,7 +12125,7 @@
       <c r="I124" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="J124" s="15">
+      <c r="J124" s="2">
         <v>40</v>
       </c>
       <c r="K124" s="5" t="s">
@@ -12213,7 +12205,7 @@
       <c r="I125" s="3">
         <v>30403</v>
       </c>
-      <c r="J125" s="15">
+      <c r="J125" s="2">
         <v>41</v>
       </c>
       <c r="K125" s="5" t="s">
@@ -12291,7 +12283,7 @@
       <c r="I126" s="3">
         <v>36161</v>
       </c>
-      <c r="J126" s="15">
+      <c r="J126" s="2">
         <v>25</v>
       </c>
       <c r="K126" s="5" t="s">
@@ -12371,7 +12363,7 @@
       <c r="I127" s="3">
         <v>31632</v>
       </c>
-      <c r="J127" s="15">
+      <c r="J127" s="2">
         <v>37</v>
       </c>
       <c r="K127" s="5" t="s">
@@ -12451,7 +12443,7 @@
       <c r="I128" s="3">
         <v>30724</v>
       </c>
-      <c r="J128" s="15">
+      <c r="J128" s="2">
         <v>40</v>
       </c>
       <c r="K128" s="5" t="s">
@@ -12531,7 +12523,7 @@
       <c r="I129" s="3">
         <v>28930</v>
       </c>
-      <c r="J129" s="15">
+      <c r="J129" s="2">
         <v>45</v>
       </c>
       <c r="K129" s="5" t="s">
@@ -12611,7 +12603,7 @@
       <c r="I130" s="3">
         <v>29015</v>
       </c>
-      <c r="J130" s="15">
+      <c r="J130" s="2">
         <v>45</v>
       </c>
       <c r="K130" s="5" t="s">
@@ -12687,7 +12679,7 @@
       <c r="I131" s="3">
         <v>36642</v>
       </c>
-      <c r="J131" s="15">
+      <c r="J131" s="2">
         <v>23</v>
       </c>
       <c r="K131" s="5" t="s">
@@ -12767,7 +12759,7 @@
       <c r="I132" s="3">
         <v>30017</v>
       </c>
-      <c r="J132" s="15">
+      <c r="J132" s="2">
         <v>41</v>
       </c>
       <c r="K132" s="5" t="s">
@@ -12847,7 +12839,7 @@
       <c r="I133" s="3">
         <v>31710</v>
       </c>
-      <c r="J133" s="15">
+      <c r="J133" s="2">
         <v>37</v>
       </c>
       <c r="K133" s="5" t="s">
@@ -12925,7 +12917,7 @@
       <c r="I134" s="3">
         <v>35069</v>
       </c>
-      <c r="J134" s="15">
+      <c r="J134" s="2">
         <v>28</v>
       </c>
       <c r="K134" s="5" t="s">
@@ -13003,7 +12995,7 @@
       <c r="I135" s="3">
         <v>37243</v>
       </c>
-      <c r="J135" s="15">
+      <c r="J135" s="2">
         <v>22</v>
       </c>
       <c r="K135" s="5" t="s">
@@ -13081,7 +13073,7 @@
       <c r="I136" s="3">
         <v>33235</v>
       </c>
-      <c r="J136" s="15">
+      <c r="J136" s="2">
         <v>33</v>
       </c>
       <c r="K136" s="5" t="s">
@@ -13159,7 +13151,7 @@
       <c r="I137" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="J137" s="15">
+      <c r="J137" s="2">
         <v>45</v>
       </c>
       <c r="K137" s="5" t="s">
@@ -13237,7 +13229,7 @@
       <c r="I138" s="3">
         <v>31660</v>
       </c>
-      <c r="J138" s="15">
+      <c r="J138" s="2">
         <v>37</v>
       </c>
       <c r="K138" s="5" t="s">
@@ -13315,7 +13307,7 @@
       <c r="I139" s="3">
         <v>29871</v>
       </c>
-      <c r="J139" s="15">
+      <c r="J139" s="2">
         <v>42</v>
       </c>
       <c r="K139" s="5" t="s">
@@ -13393,7 +13385,7 @@
       <c r="I140" s="3">
         <v>32450</v>
       </c>
-      <c r="J140" s="15">
+      <c r="J140" s="2">
         <v>35</v>
       </c>
       <c r="K140" s="5" t="s">
@@ -13471,7 +13463,7 @@
       <c r="I141" s="3">
         <v>32138</v>
       </c>
-      <c r="J141" s="15">
+      <c r="J141" s="2">
         <v>36</v>
       </c>
       <c r="K141" s="5" t="s">
@@ -13549,7 +13541,7 @@
       <c r="I142" s="3">
         <v>30856</v>
       </c>
-      <c r="J142" s="15">
+      <c r="J142" s="2">
         <v>39</v>
       </c>
       <c r="K142" s="5" t="s">
@@ -13627,7 +13619,7 @@
       <c r="I143" s="3">
         <v>30312</v>
       </c>
-      <c r="J143" s="15">
+      <c r="J143" s="2">
         <v>41</v>
       </c>
       <c r="K143" s="5" t="s">
@@ -13705,7 +13697,7 @@
       <c r="I144" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="J144" s="15">
+      <c r="J144" s="2">
         <v>44</v>
       </c>
       <c r="K144" s="5" t="s">
@@ -13783,7 +13775,7 @@
       <c r="I145" s="3">
         <v>36195</v>
       </c>
-      <c r="J145" s="15">
+      <c r="J145" s="2">
         <v>25</v>
       </c>
       <c r="K145" s="5" t="s">
@@ -13861,7 +13853,7 @@
       <c r="I146" s="3">
         <v>33565</v>
       </c>
-      <c r="J146" s="15">
+      <c r="J146" s="2">
         <v>32</v>
       </c>
       <c r="K146" s="5" t="s">
@@ -13939,7 +13931,7 @@
       <c r="I147" s="3">
         <v>31569</v>
       </c>
-      <c r="J147" s="15">
+      <c r="J147" s="2">
         <v>38</v>
       </c>
       <c r="K147" s="5" t="s">
@@ -14017,7 +14009,7 @@
       <c r="I148" s="3">
         <v>1</v>
       </c>
-      <c r="J148" s="15">
+      <c r="J148" s="2">
         <v>124</v>
       </c>
       <c r="K148" s="5" t="s">
@@ -14095,7 +14087,7 @@
       <c r="I149" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="J149" s="15">
+      <c r="J149" s="2">
         <v>36</v>
       </c>
       <c r="K149" s="5" t="s">
@@ -14173,7 +14165,7 @@
       <c r="I150" s="3">
         <v>32128</v>
       </c>
-      <c r="J150" s="15">
+      <c r="J150" s="2">
         <v>36</v>
       </c>
       <c r="K150" s="5" t="s">
@@ -14251,7 +14243,7 @@
       <c r="I151" s="3">
         <v>35377</v>
       </c>
-      <c r="J151" s="15">
+      <c r="J151" s="2">
         <v>27</v>
       </c>
       <c r="K151" s="5" t="s">
@@ -14329,7 +14321,7 @@
       <c r="I152" s="3">
         <v>32731</v>
       </c>
-      <c r="J152" s="15">
+      <c r="J152" s="2">
         <v>35</v>
       </c>
       <c r="K152" s="5" t="s">
@@ -14407,7 +14399,7 @@
       <c r="I153" s="3">
         <v>36532</v>
       </c>
-      <c r="J153" s="15">
+      <c r="J153" s="2">
         <v>24</v>
       </c>
       <c r="K153" s="5" t="s">
@@ -14485,7 +14477,7 @@
       <c r="I154" s="3">
         <v>35944</v>
       </c>
-      <c r="J154" s="15">
+      <c r="J154" s="2">
         <v>26</v>
       </c>
       <c r="K154" s="5" t="s">
@@ -14563,7 +14555,7 @@
       <c r="I155" s="3">
         <v>26542</v>
       </c>
-      <c r="J155" s="15">
+      <c r="J155" s="2">
         <v>52</v>
       </c>
       <c r="K155" s="5" t="s">
@@ -14641,7 +14633,7 @@
       <c r="I156" s="3">
         <v>32550</v>
       </c>
-      <c r="J156" s="15">
+      <c r="J156" s="2">
         <v>35</v>
       </c>
       <c r="K156" s="5" t="s">
@@ -14719,7 +14711,7 @@
       <c r="I157" s="3">
         <v>32505</v>
       </c>
-      <c r="J157" s="15">
+      <c r="J157" s="2">
         <v>35</v>
       </c>
       <c r="K157" s="5" t="s">
@@ -14797,7 +14789,7 @@
       <c r="I158" s="3">
         <v>35150</v>
       </c>
-      <c r="J158" s="15">
+      <c r="J158" s="2">
         <v>28</v>
       </c>
       <c r="K158" s="5" t="s">
@@ -14875,7 +14867,7 @@
       <c r="I159" s="3">
         <v>37355</v>
       </c>
-      <c r="J159" s="15">
+      <c r="J159" s="2">
         <v>22</v>
       </c>
       <c r="K159" s="5" t="s">
@@ -14951,7 +14943,7 @@
       <c r="I160" s="3">
         <v>36127</v>
       </c>
-      <c r="J160" s="15">
+      <c r="J160" s="2">
         <v>25</v>
       </c>
       <c r="K160" s="5" t="s">
@@ -15027,7 +15019,7 @@
       <c r="I161" s="3">
         <v>26665</v>
       </c>
-      <c r="J161" s="15">
+      <c r="J161" s="2">
         <v>51</v>
       </c>
       <c r="K161" s="5" t="s">
@@ -15103,7 +15095,7 @@
       <c r="I162" s="3">
         <v>31407</v>
       </c>
-      <c r="J162" s="15">
+      <c r="J162" s="2">
         <v>38</v>
       </c>
       <c r="K162" s="5" t="s">
@@ -15179,7 +15171,7 @@
       <c r="I163" s="3">
         <v>33574</v>
       </c>
-      <c r="J163" s="15">
+      <c r="J163" s="2">
         <v>31</v>
       </c>
       <c r="K163" s="5" t="s">
@@ -15255,7 +15247,7 @@
       <c r="I164" s="3">
         <v>32124</v>
       </c>
-      <c r="J164" s="15">
+      <c r="J164" s="2">
         <v>34</v>
       </c>
       <c r="K164" s="5" t="s">
@@ -15331,7 +15323,7 @@
       <c r="I165" s="3">
         <v>30317</v>
       </c>
-      <c r="J165" s="15">
+      <c r="J165" s="2">
         <v>41</v>
       </c>
       <c r="K165" s="5" t="s">
@@ -15407,7 +15399,7 @@
       <c r="I166" s="3">
         <v>33598</v>
       </c>
-      <c r="J166" s="15">
+      <c r="J166" s="2">
         <v>32</v>
       </c>
       <c r="K166" s="5" t="s">
@@ -15483,7 +15475,7 @@
       <c r="I167" s="3">
         <v>32229</v>
       </c>
-      <c r="J167" s="15">
+      <c r="J167" s="2">
         <v>36</v>
       </c>
       <c r="K167" s="5" t="s">
@@ -15559,7 +15551,7 @@
       <c r="I168" s="3">
         <v>33273</v>
       </c>
-      <c r="J168" s="15">
+      <c r="J168" s="2">
         <v>33</v>
       </c>
       <c r="K168" s="5" t="s">
@@ -15635,7 +15627,7 @@
       <c r="I169" s="3">
         <v>27794</v>
       </c>
-      <c r="J169" s="15">
+      <c r="J169" s="2">
         <v>48</v>
       </c>
       <c r="K169" s="5" t="s">
@@ -15711,7 +15703,7 @@
       <c r="I170" s="3">
         <v>31631</v>
       </c>
-      <c r="J170" s="15">
+      <c r="J170" s="2">
         <v>38</v>
       </c>
       <c r="K170" s="5" t="s">
@@ -15787,7 +15779,7 @@
       <c r="I171" s="3">
         <v>28487</v>
       </c>
-      <c r="J171" s="15">
+      <c r="J171" s="2">
         <v>46</v>
       </c>
       <c r="K171" s="5" t="s">
@@ -15863,7 +15855,7 @@
       <c r="I172" s="3">
         <v>32883</v>
       </c>
-      <c r="J172" s="15">
+      <c r="J172" s="2">
         <v>34</v>
       </c>
       <c r="K172" s="5" t="s">
@@ -15932,10 +15924,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="11" style="16"/>
-    <col min="3" max="3" width="11" style="16"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1">
@@ -15944,7 +15932,7 @@
       <c r="B1" s="1">
         <v>45230</v>
       </c>
-      <c r="C1" s="16">
+      <c r="C1">
         <f>DATEDIF(A1, B1, "Y")</f>
         <v>41</v>
       </c>
@@ -15956,7 +15944,7 @@
       <c r="B2" s="1">
         <v>44758</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2">
         <f t="shared" ref="C2:C65" si="0">DATEDIF(A2, B2, "Y")</f>
         <v>28</v>
       </c>
@@ -15968,7 +15956,7 @@
       <c r="B3" s="1">
         <v>44758</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
@@ -15980,7 +15968,7 @@
       <c r="B4" s="1">
         <v>45192</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
@@ -15992,7 +15980,7 @@
       <c r="B5" s="1">
         <v>45288</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
@@ -16004,7 +15992,7 @@
       <c r="B6" s="1">
         <v>45259</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
@@ -16016,7 +16004,7 @@
       <c r="B7" s="1">
         <v>45281</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
@@ -16028,7 +16016,7 @@
       <c r="B8" s="1">
         <v>45296</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
@@ -16040,7 +16028,7 @@
       <c r="B9" s="1">
         <v>45284</v>
       </c>
-      <c r="C9" s="16" t="e">
+      <c r="C9" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
@@ -16052,7 +16040,7 @@
       <c r="B10" s="1">
         <v>45238</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
@@ -16064,7 +16052,7 @@
       <c r="B11" s="1">
         <v>45217</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
@@ -16076,7 +16064,7 @@
       <c r="B12" s="1">
         <v>44994</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
@@ -16088,7 +16076,7 @@
       <c r="B13" s="1">
         <v>45096</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
@@ -16100,7 +16088,7 @@
       <c r="B14" s="1">
         <v>45163</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14">
         <f t="shared" si="0"/>
         <v>123</v>
       </c>
@@ -16112,7 +16100,7 @@
       <c r="B15" s="1">
         <v>45288</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
@@ -16124,7 +16112,7 @@
       <c r="B16" s="1">
         <v>45271</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
@@ -16136,7 +16124,7 @@
       <c r="B17" s="1">
         <v>45271</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
@@ -16148,7 +16136,7 @@
       <c r="B18" s="1">
         <v>45271</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
@@ -16160,7 +16148,7 @@
       <c r="B19" s="1">
         <v>45271</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -16172,7 +16160,7 @@
       <c r="B20" s="1">
         <v>45183</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C20">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
@@ -16184,7 +16172,7 @@
       <c r="B21" s="1">
         <v>45200</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C21">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
@@ -16196,7 +16184,7 @@
       <c r="B22" s="1">
         <v>43929</v>
       </c>
-      <c r="C22" s="16">
+      <c r="C22">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -16208,7 +16196,7 @@
       <c r="B23" s="1">
         <v>45287</v>
       </c>
-      <c r="C23" s="16">
+      <c r="C23">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -16220,7 +16208,7 @@
       <c r="B24" s="1">
         <v>45017</v>
       </c>
-      <c r="C24" s="16">
+      <c r="C24">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
@@ -16232,7 +16220,7 @@
       <c r="B25" s="1">
         <v>45279</v>
       </c>
-      <c r="C25" s="16">
+      <c r="C25">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
@@ -16244,7 +16232,7 @@
       <c r="B26" s="1">
         <v>45175</v>
       </c>
-      <c r="C26" s="16">
+      <c r="C26">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
@@ -16256,7 +16244,7 @@
       <c r="B27" s="1">
         <v>45175</v>
       </c>
-      <c r="C27" s="16">
+      <c r="C27">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
@@ -16268,7 +16256,7 @@
       <c r="B28" s="1">
         <v>45199</v>
       </c>
-      <c r="C28" s="16">
+      <c r="C28">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
@@ -16280,7 +16268,7 @@
       <c r="B29" s="1">
         <v>45288</v>
       </c>
-      <c r="C29" s="16">
+      <c r="C29">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
@@ -16292,7 +16280,7 @@
       <c r="B30" s="1">
         <v>44931</v>
       </c>
-      <c r="C30" s="16">
+      <c r="C30">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
@@ -16304,7 +16292,7 @@
       <c r="B31" s="1">
         <v>45066</v>
       </c>
-      <c r="C31" s="16">
+      <c r="C31">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
@@ -16316,7 +16304,7 @@
       <c r="B32" s="1">
         <v>45066</v>
       </c>
-      <c r="C32" s="16">
+      <c r="C32">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
@@ -16328,7 +16316,7 @@
       <c r="B33" s="1">
         <v>45066</v>
       </c>
-      <c r="C33" s="16">
+      <c r="C33">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
@@ -16340,7 +16328,7 @@
       <c r="B34" s="1">
         <v>45066</v>
       </c>
-      <c r="C34" s="16">
+      <c r="C34">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
@@ -16352,7 +16340,7 @@
       <c r="B35" s="1">
         <v>45149</v>
       </c>
-      <c r="C35" s="16">
+      <c r="C35">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
@@ -16364,7 +16352,7 @@
       <c r="B36" s="1">
         <v>45210</v>
       </c>
-      <c r="C36" s="16">
+      <c r="C36">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
@@ -16376,7 +16364,7 @@
       <c r="B37" s="1">
         <v>45287</v>
       </c>
-      <c r="C37" s="16">
+      <c r="C37">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
@@ -16388,7 +16376,7 @@
       <c r="B38" s="1">
         <v>45275</v>
       </c>
-      <c r="C38" s="16">
+      <c r="C38">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
@@ -16400,7 +16388,7 @@
       <c r="B39" s="1">
         <v>45159</v>
       </c>
-      <c r="C39" s="16">
+      <c r="C39">
         <f t="shared" si="0"/>
         <v>123</v>
       </c>
@@ -16412,7 +16400,7 @@
       <c r="B40" s="1">
         <v>45276</v>
       </c>
-      <c r="C40" s="16">
+      <c r="C40">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
@@ -16424,7 +16412,7 @@
       <c r="B41" s="1">
         <v>45292</v>
       </c>
-      <c r="C41" s="16">
+      <c r="C41">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
@@ -16436,7 +16424,7 @@
       <c r="B42" s="1">
         <v>45292</v>
       </c>
-      <c r="C42" s="16">
+      <c r="C42">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
@@ -16448,7 +16436,7 @@
       <c r="B43" s="1">
         <v>45292</v>
       </c>
-      <c r="C43" s="16">
+      <c r="C43">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
@@ -16460,7 +16448,7 @@
       <c r="B44" s="1">
         <v>45292</v>
       </c>
-      <c r="C44" s="16">
+      <c r="C44">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
@@ -16472,7 +16460,7 @@
       <c r="B45" s="1">
         <v>45237</v>
       </c>
-      <c r="C45" s="16">
+      <c r="C45">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
@@ -16484,7 +16472,7 @@
       <c r="B46" s="1">
         <v>45268</v>
       </c>
-      <c r="C46" s="16">
+      <c r="C46">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
@@ -16496,7 +16484,7 @@
       <c r="B47" s="1">
         <v>44773</v>
       </c>
-      <c r="C47" s="16">
+      <c r="C47">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
@@ -16508,7 +16496,7 @@
       <c r="B48" s="1">
         <v>45215</v>
       </c>
-      <c r="C48" s="16">
+      <c r="C48">
         <f t="shared" si="0"/>
         <v>123</v>
       </c>
@@ -16520,7 +16508,7 @@
       <c r="B49" s="1">
         <v>45293</v>
       </c>
-      <c r="C49" s="16">
+      <c r="C49">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
@@ -16532,7 +16520,7 @@
       <c r="B50" s="1">
         <v>45258</v>
       </c>
-      <c r="C50" s="16">
+      <c r="C50">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
@@ -16544,7 +16532,7 @@
       <c r="B51" s="1">
         <v>45172</v>
       </c>
-      <c r="C51" s="16">
+      <c r="C51">
         <f t="shared" si="0"/>
         <v>123</v>
       </c>
@@ -16556,7 +16544,7 @@
       <c r="B52" s="1">
         <v>45282</v>
       </c>
-      <c r="C52" s="16">
+      <c r="C52">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
@@ -16568,7 +16556,7 @@
       <c r="B53" s="1">
         <v>45225</v>
       </c>
-      <c r="C53" s="16">
+      <c r="C53">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
@@ -16580,7 +16568,7 @@
       <c r="B54" s="1">
         <v>45304</v>
       </c>
-      <c r="C54" s="16">
+      <c r="C54">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
@@ -16592,7 +16580,7 @@
       <c r="B55" s="1">
         <v>45334</v>
       </c>
-      <c r="C55" s="16">
+      <c r="C55">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
@@ -16604,7 +16592,7 @@
       <c r="B56" s="1">
         <v>45212</v>
       </c>
-      <c r="C56" s="16">
+      <c r="C56">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
@@ -16616,7 +16604,7 @@
       <c r="B57" s="1">
         <v>45340</v>
       </c>
-      <c r="C57" s="16">
+      <c r="C57">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
@@ -16628,7 +16616,7 @@
       <c r="B58" s="1">
         <v>45183</v>
       </c>
-      <c r="C58" s="16">
+      <c r="C58">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
@@ -16640,7 +16628,7 @@
       <c r="B59" s="1">
         <v>45637</v>
       </c>
-      <c r="C59" s="16">
+      <c r="C59">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
@@ -16652,7 +16640,7 @@
       <c r="B60" s="1">
         <v>45351</v>
       </c>
-      <c r="C60" s="16">
+      <c r="C60">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
@@ -16664,7 +16652,7 @@
       <c r="B61" s="1">
         <v>45356</v>
       </c>
-      <c r="C61" s="16">
+      <c r="C61">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
@@ -16676,7 +16664,7 @@
       <c r="B62" s="1">
         <v>45356</v>
       </c>
-      <c r="C62" s="16">
+      <c r="C62">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
@@ -16688,7 +16676,7 @@
       <c r="B63" s="1">
         <v>45356</v>
       </c>
-      <c r="C63" s="16">
+      <c r="C63">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
@@ -16700,7 +16688,7 @@
       <c r="B64" s="1">
         <v>45356</v>
       </c>
-      <c r="C64" s="16">
+      <c r="C64">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
@@ -16712,7 +16700,7 @@
       <c r="B65" s="1">
         <v>45356</v>
       </c>
-      <c r="C65" s="16">
+      <c r="C65">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
@@ -16724,7 +16712,7 @@
       <c r="B66" s="1">
         <v>45356</v>
       </c>
-      <c r="C66" s="16">
+      <c r="C66">
         <f t="shared" ref="C66:C129" si="1">DATEDIF(A66, B66, "Y")</f>
         <v>24</v>
       </c>
@@ -16736,7 +16724,7 @@
       <c r="B67" s="1">
         <v>45356</v>
       </c>
-      <c r="C67" s="16">
+      <c r="C67">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
@@ -16748,7 +16736,7 @@
       <c r="B68" s="1">
         <v>45224</v>
       </c>
-      <c r="C68" s="16">
+      <c r="C68">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
@@ -16760,7 +16748,7 @@
       <c r="B69" s="1">
         <v>40179</v>
       </c>
-      <c r="C69" s="16">
+      <c r="C69">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
@@ -16772,7 +16760,7 @@
       <c r="B70" s="1">
         <v>45376</v>
       </c>
-      <c r="C70" s="16">
+      <c r="C70">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
@@ -16784,7 +16772,7 @@
       <c r="B71" s="1">
         <v>45374</v>
       </c>
-      <c r="C71" s="16">
+      <c r="C71">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
@@ -16796,7 +16784,7 @@
       <c r="B72" s="1">
         <v>45374</v>
       </c>
-      <c r="C72" s="16">
+      <c r="C72">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
@@ -16808,7 +16796,7 @@
       <c r="B73" s="1">
         <v>43865</v>
       </c>
-      <c r="C73" s="16">
+      <c r="C73">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
@@ -16820,7 +16808,7 @@
       <c r="B74" s="1">
         <v>45352</v>
       </c>
-      <c r="C74" s="16">
+      <c r="C74">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
@@ -16832,7 +16820,7 @@
       <c r="B75" s="1">
         <v>44081</v>
       </c>
-      <c r="C75" s="16">
+      <c r="C75">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
@@ -16844,7 +16832,7 @@
       <c r="B76" s="1">
         <v>45374</v>
       </c>
-      <c r="C76" s="16">
+      <c r="C76">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
@@ -16856,7 +16844,7 @@
       <c r="B77" s="1">
         <v>45268</v>
       </c>
-      <c r="C77" s="16">
+      <c r="C77">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
@@ -16868,7 +16856,7 @@
       <c r="B78" s="1">
         <v>45262</v>
       </c>
-      <c r="C78" s="16">
+      <c r="C78">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
@@ -16880,7 +16868,7 @@
       <c r="B79" s="1">
         <v>45319</v>
       </c>
-      <c r="C79" s="16">
+      <c r="C79">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
@@ -16892,7 +16880,7 @@
       <c r="B80" s="1">
         <v>45254</v>
       </c>
-      <c r="C80" s="16">
+      <c r="C80">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
@@ -16904,7 +16892,7 @@
       <c r="B81" s="1">
         <v>45206</v>
       </c>
-      <c r="C81" s="16">
+      <c r="C81">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
@@ -16916,7 +16904,7 @@
       <c r="B82" s="1">
         <v>45359</v>
       </c>
-      <c r="C82" s="16">
+      <c r="C82">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
@@ -16928,7 +16916,7 @@
       <c r="B83" s="1">
         <v>45322</v>
       </c>
-      <c r="C83" s="16">
+      <c r="C83">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
@@ -16940,7 +16928,7 @@
       <c r="B84" s="1">
         <v>45399</v>
       </c>
-      <c r="C84" s="16">
+      <c r="C84">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
@@ -16952,7 +16940,7 @@
       <c r="B85" s="1">
         <v>45399</v>
       </c>
-      <c r="C85" s="16">
+      <c r="C85">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
@@ -16964,7 +16952,7 @@
       <c r="B86" s="1">
         <v>45339</v>
       </c>
-      <c r="C86" s="16">
+      <c r="C86">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
@@ -16976,7 +16964,7 @@
       <c r="B87" s="1">
         <v>45340</v>
       </c>
-      <c r="C87" s="16">
+      <c r="C87">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
@@ -16988,7 +16976,7 @@
       <c r="B88" s="1">
         <v>45405</v>
       </c>
-      <c r="C88" s="16">
+      <c r="C88">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
@@ -17000,7 +16988,7 @@
       <c r="B89" s="1">
         <v>45167</v>
       </c>
-      <c r="C89" s="16">
+      <c r="C89">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
@@ -17012,7 +17000,7 @@
       <c r="B90" s="1">
         <v>45245</v>
       </c>
-      <c r="C90" s="16">
+      <c r="C90">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
@@ -17024,7 +17012,7 @@
       <c r="B91" s="1">
         <v>45278</v>
       </c>
-      <c r="C91" s="16">
+      <c r="C91">
         <f t="shared" si="1"/>
         <v>123</v>
       </c>
@@ -17036,7 +17024,7 @@
       <c r="B92" s="1">
         <v>45351</v>
       </c>
-      <c r="C92" s="16">
+      <c r="C92">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
@@ -17048,7 +17036,7 @@
       <c r="B93" s="1">
         <v>45351</v>
       </c>
-      <c r="C93" s="16">
+      <c r="C93">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
@@ -17060,7 +17048,7 @@
       <c r="B94" s="1">
         <v>45360</v>
       </c>
-      <c r="C94" s="16">
+      <c r="C94">
         <f t="shared" si="1"/>
         <v>124</v>
       </c>
@@ -17072,7 +17060,7 @@
       <c r="B95" s="1">
         <v>45231</v>
       </c>
-      <c r="C95" s="16">
+      <c r="C95">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
@@ -17084,7 +17072,7 @@
       <c r="B96" s="1">
         <v>45382</v>
       </c>
-      <c r="C96" s="16">
+      <c r="C96">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
@@ -17096,7 +17084,7 @@
       <c r="B97" s="1">
         <v>45393</v>
       </c>
-      <c r="C97" s="16">
+      <c r="C97">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
@@ -17108,7 +17096,7 @@
       <c r="B98" s="1">
         <v>45383</v>
       </c>
-      <c r="C98" s="16">
+      <c r="C98">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
@@ -17120,7 +17108,7 @@
       <c r="B99" s="1">
         <v>45391</v>
       </c>
-      <c r="C99" s="16">
+      <c r="C99">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
@@ -17132,7 +17120,7 @@
       <c r="B100" s="1">
         <v>45390</v>
       </c>
-      <c r="C100" s="16">
+      <c r="C100">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
@@ -17144,7 +17132,7 @@
       <c r="B101" s="1">
         <v>45421</v>
       </c>
-      <c r="C101" s="16">
+      <c r="C101">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
@@ -17156,7 +17144,7 @@
       <c r="B102" s="1">
         <v>45413</v>
       </c>
-      <c r="C102" s="16">
+      <c r="C102">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
@@ -17168,7 +17156,7 @@
       <c r="B103" s="1">
         <v>45397</v>
       </c>
-      <c r="C103" s="16">
+      <c r="C103">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
@@ -17180,7 +17168,7 @@
       <c r="B104" s="1">
         <v>45440</v>
       </c>
-      <c r="C104" s="16">
+      <c r="C104">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
@@ -17192,7 +17180,7 @@
       <c r="B105" s="1">
         <v>45394</v>
       </c>
-      <c r="C105" s="16">
+      <c r="C105">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
@@ -17204,7 +17192,7 @@
       <c r="B106" s="1">
         <v>45396</v>
       </c>
-      <c r="C106" s="16">
+      <c r="C106">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
@@ -17216,7 +17204,7 @@
       <c r="B107" s="1">
         <v>45443</v>
       </c>
-      <c r="C107" s="16">
+      <c r="C107">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
@@ -17228,7 +17216,7 @@
       <c r="B108" s="1">
         <v>45436</v>
       </c>
-      <c r="C108" s="16">
+      <c r="C108">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
@@ -17240,7 +17228,7 @@
       <c r="B109" s="1">
         <v>45017</v>
       </c>
-      <c r="C109" s="16">
+      <c r="C109">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
@@ -17252,7 +17240,7 @@
       <c r="B110" s="1">
         <v>43771</v>
       </c>
-      <c r="C110" s="16">
+      <c r="C110">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
@@ -17264,7 +17252,7 @@
       <c r="B111" s="1">
         <v>45480</v>
       </c>
-      <c r="C111" s="16">
+      <c r="C111">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
@@ -17276,7 +17264,7 @@
       <c r="B112" s="1">
         <v>45450</v>
       </c>
-      <c r="C112" s="16">
+      <c r="C112">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
@@ -17288,7 +17276,7 @@
       <c r="B113" s="1">
         <v>45427</v>
       </c>
-      <c r="C113" s="16">
+      <c r="C113">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
@@ -17300,7 +17288,7 @@
       <c r="B114" s="1">
         <v>44562</v>
       </c>
-      <c r="C114" s="16">
+      <c r="C114">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
@@ -17312,7 +17300,7 @@
       <c r="B115" s="1">
         <v>45387</v>
       </c>
-      <c r="C115" s="16">
+      <c r="C115">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
@@ -17324,7 +17312,7 @@
       <c r="B116" s="1">
         <v>45414</v>
       </c>
-      <c r="C116" s="16">
+      <c r="C116">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
@@ -17336,7 +17324,7 @@
       <c r="B117" s="1">
         <v>45294</v>
       </c>
-      <c r="C117" s="16">
+      <c r="C117">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
@@ -17348,7 +17336,7 @@
       <c r="B118" s="1">
         <v>43743</v>
       </c>
-      <c r="C118" s="16">
+      <c r="C118">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
@@ -17360,7 +17348,7 @@
       <c r="B119" s="1">
         <v>45437</v>
       </c>
-      <c r="C119" s="16">
+      <c r="C119">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
@@ -17372,7 +17360,7 @@
       <c r="B120" s="1">
         <v>45047</v>
       </c>
-      <c r="C120" s="16">
+      <c r="C120">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
@@ -17384,7 +17372,7 @@
       <c r="B121" s="1">
         <v>45466</v>
       </c>
-      <c r="C121" s="16">
+      <c r="C121">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
@@ -17396,7 +17384,7 @@
       <c r="B122" s="1">
         <v>45287</v>
       </c>
-      <c r="C122" s="16">
+      <c r="C122">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
@@ -17408,7 +17396,7 @@
       <c r="B123" s="1">
         <v>45111</v>
       </c>
-      <c r="C123" s="16">
+      <c r="C123">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
@@ -17420,7 +17408,7 @@
       <c r="B124" s="1">
         <v>45482</v>
       </c>
-      <c r="C124" s="16">
+      <c r="C124">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
@@ -17432,7 +17420,7 @@
       <c r="B125" s="1">
         <v>45485</v>
       </c>
-      <c r="C125" s="16">
+      <c r="C125">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
@@ -17444,7 +17432,7 @@
       <c r="B126" s="1">
         <v>45221</v>
       </c>
-      <c r="C126" s="16">
+      <c r="C126">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
@@ -17456,7 +17444,7 @@
       <c r="B127" s="1">
         <v>45442</v>
       </c>
-      <c r="C127" s="16">
+      <c r="C127">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
@@ -17468,7 +17456,7 @@
       <c r="B128" s="1">
         <v>45442</v>
       </c>
-      <c r="C128" s="16">
+      <c r="C128">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
@@ -17480,7 +17468,7 @@
       <c r="B129" s="1">
         <v>45500</v>
       </c>
-      <c r="C129" s="16">
+      <c r="C129">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
@@ -17492,7 +17480,7 @@
       <c r="B130" s="1">
         <v>45267</v>
       </c>
-      <c r="C130" s="16">
+      <c r="C130">
         <f t="shared" ref="C130:C172" si="2">DATEDIF(A130, B130, "Y")</f>
         <v>23</v>
       </c>
@@ -17504,7 +17492,7 @@
       <c r="B131" s="1">
         <v>45281</v>
       </c>
-      <c r="C131" s="16">
+      <c r="C131">
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
@@ -17516,7 +17504,7 @@
       <c r="B132" s="1">
         <v>45477</v>
       </c>
-      <c r="C132" s="16">
+      <c r="C132">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
@@ -17528,7 +17516,7 @@
       <c r="B133" s="1">
         <v>45397</v>
       </c>
-      <c r="C133" s="16">
+      <c r="C133">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
@@ -17540,7 +17528,7 @@
       <c r="B134" s="1">
         <v>45467</v>
       </c>
-      <c r="C134" s="16">
+      <c r="C134">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
@@ -17552,7 +17540,7 @@
       <c r="B135" s="1">
         <v>45497</v>
       </c>
-      <c r="C135" s="16">
+      <c r="C135">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
@@ -17564,7 +17552,7 @@
       <c r="B136" s="1">
         <v>45497</v>
       </c>
-      <c r="C136" s="16">
+      <c r="C136">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
@@ -17576,7 +17564,7 @@
       <c r="B137" s="1">
         <v>45497</v>
       </c>
-      <c r="C137" s="16">
+      <c r="C137">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
@@ -17588,7 +17576,7 @@
       <c r="B138" s="1">
         <v>45523</v>
       </c>
-      <c r="C138" s="16">
+      <c r="C138">
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
@@ -17600,7 +17588,7 @@
       <c r="B139" s="1">
         <v>45507</v>
       </c>
-      <c r="C139" s="16">
+      <c r="C139">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
@@ -17612,7 +17600,7 @@
       <c r="B140" s="1">
         <v>45456</v>
       </c>
-      <c r="C140" s="16">
+      <c r="C140">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
@@ -17624,7 +17612,7 @@
       <c r="B141" s="1">
         <v>45425</v>
       </c>
-      <c r="C141" s="16">
+      <c r="C141">
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
@@ -17636,7 +17624,7 @@
       <c r="B142" s="1">
         <v>45537</v>
       </c>
-      <c r="C142" s="16">
+      <c r="C142">
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
@@ -17648,7 +17636,7 @@
       <c r="B143" s="1">
         <v>45523</v>
       </c>
-      <c r="C143" s="16">
+      <c r="C143">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
@@ -17660,7 +17648,7 @@
       <c r="B144" s="1">
         <v>45503</v>
       </c>
-      <c r="C144" s="16">
+      <c r="C144">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
@@ -17672,7 +17660,7 @@
       <c r="B145" s="1">
         <v>45454</v>
       </c>
-      <c r="C145" s="16">
+      <c r="C145">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
@@ -17684,7 +17672,7 @@
       <c r="B146" s="1">
         <v>45537</v>
       </c>
-      <c r="C146" s="16">
+      <c r="C146">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
@@ -17696,7 +17684,7 @@
       <c r="B147" s="1">
         <v>45537</v>
       </c>
-      <c r="C147" s="16">
+      <c r="C147">
         <f t="shared" si="2"/>
         <v>124</v>
       </c>
@@ -17708,7 +17696,7 @@
       <c r="B148" s="1">
         <v>45277</v>
       </c>
-      <c r="C148" s="16">
+      <c r="C148">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
@@ -17720,7 +17708,7 @@
       <c r="B149" s="1">
         <v>45519</v>
       </c>
-      <c r="C149" s="16">
+      <c r="C149">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
@@ -17732,7 +17720,7 @@
       <c r="B150" s="1">
         <v>45470</v>
       </c>
-      <c r="C150" s="16">
+      <c r="C150">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
@@ -17744,7 +17732,7 @@
       <c r="B151" s="1">
         <v>45558</v>
       </c>
-      <c r="C151" s="16">
+      <c r="C151">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
@@ -17756,7 +17744,7 @@
       <c r="B152" s="1">
         <v>45490</v>
       </c>
-      <c r="C152" s="16">
+      <c r="C152">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
@@ -17768,7 +17756,7 @@
       <c r="B153" s="1">
         <v>45516</v>
       </c>
-      <c r="C153" s="16">
+      <c r="C153">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
@@ -17780,7 +17768,7 @@
       <c r="B154" s="1">
         <v>45551</v>
       </c>
-      <c r="C154" s="16">
+      <c r="C154">
         <f t="shared" si="2"/>
         <v>52</v>
       </c>
@@ -17792,7 +17780,7 @@
       <c r="B155" s="1">
         <v>45531</v>
       </c>
-      <c r="C155" s="16">
+      <c r="C155">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
@@ -17804,7 +17792,7 @@
       <c r="B156" s="1">
         <v>45490</v>
       </c>
-      <c r="C156" s="16">
+      <c r="C156">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
@@ -17816,7 +17804,7 @@
       <c r="B157" s="1">
         <v>45558</v>
       </c>
-      <c r="C157" s="16">
+      <c r="C157">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
@@ -17828,7 +17816,7 @@
       <c r="B158" s="1">
         <v>45563</v>
       </c>
-      <c r="C158" s="16">
+      <c r="C158">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
@@ -17840,7 +17828,7 @@
       <c r="B159" s="1">
         <v>45434</v>
       </c>
-      <c r="C159" s="16">
+      <c r="C159">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
@@ -17852,7 +17840,7 @@
       <c r="B160" s="1">
         <v>45516</v>
       </c>
-      <c r="C160" s="16">
+      <c r="C160">
         <f t="shared" si="2"/>
         <v>51</v>
       </c>
@@ -17864,7 +17852,7 @@
       <c r="B161" s="1">
         <v>45410</v>
       </c>
-      <c r="C161" s="16">
+      <c r="C161">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
@@ -17876,7 +17864,7 @@
       <c r="B162" s="1">
         <v>45087</v>
       </c>
-      <c r="C162" s="16">
+      <c r="C162">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
@@ -17888,7 +17876,7 @@
       <c r="B163" s="1">
         <v>44691</v>
       </c>
-      <c r="C163" s="16">
+      <c r="C163">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
@@ -17900,7 +17888,7 @@
       <c r="B164" s="1">
         <v>45531</v>
       </c>
-      <c r="C164" s="16">
+      <c r="C164">
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
@@ -17912,7 +17900,7 @@
       <c r="B165" s="1">
         <v>45531</v>
       </c>
-      <c r="C165" s="16">
+      <c r="C165">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
@@ -17924,7 +17912,7 @@
       <c r="B166" s="1">
         <v>45531</v>
       </c>
-      <c r="C166" s="16">
+      <c r="C166">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
@@ -17936,7 +17924,7 @@
       <c r="B167" s="1">
         <v>45531</v>
       </c>
-      <c r="C167" s="16">
+      <c r="C167">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
@@ -17948,7 +17936,7 @@
       <c r="B168" s="1">
         <v>45555</v>
       </c>
-      <c r="C168" s="16">
+      <c r="C168">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
@@ -17960,7 +17948,7 @@
       <c r="B169" s="1">
         <v>45555</v>
       </c>
-      <c r="C169" s="16">
+      <c r="C169">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
@@ -17972,7 +17960,7 @@
       <c r="B170" s="1">
         <v>45555</v>
       </c>
-      <c r="C170" s="16">
+      <c r="C170">
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
@@ -17984,7 +17972,7 @@
       <c r="B171" s="1">
         <v>45529</v>
       </c>
-      <c r="C171" s="16">
+      <c r="C171">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
@@ -17996,7 +17984,7 @@
       <c r="B172" s="1">
         <v>45187</v>
       </c>
-      <c r="C172" s="16">
+      <c r="C172">
         <f t="shared" si="2"/>
         <v>53</v>
       </c>

</xml_diff>